<commit_message>
Modified RF. separate rest and task
</commit_message>
<xml_diff>
--- a/results/significant_networks.xlsx
+++ b/results/significant_networks.xlsx
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Medial-Occipital</t>
+          <t>Medial-Occipital_Visual</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -476,7 +476,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Occipital-Lateral(L)</t>
+          <t>Occipital-Lateral(L)_Visual</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -494,7 +494,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Medial-Lateral(L)</t>
+          <t>Medial-Lateral(L)_Visual</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -512,7 +512,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Medial-Lateral(R)</t>
+          <t>Medial-Lateral(R)_Visual</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -530,7 +530,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ACC-RPFC(L)</t>
+          <t>ACC-RPFC(L)_Salience</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -548,7 +548,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AInsula(L)-RPFC(R)</t>
+          <t>AInsula(L)-RPFC(R)_Salience</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -566,7 +566,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LPFC(L)-PPC(L)</t>
+          <t>LPFC(L)-PPC(L)_FP</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>